<commit_message>
Cambios a script de limpieza y graficos
</commit_message>
<xml_diff>
--- a/datos/crudos/ind_cantonales.xlsx
+++ b/datos/crudos/ind_cantonales.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp 15-ak006la\Dropbox\UCR\Estadistica Espacial II 2018\Proyecto-final-espacial\archivosshpycantonales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp 15-ak006la\Dropbox\UCR\Estadistica Espacial II 2018\Proyecto-final-espacial\datos\crudos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBFF86F3-6370-4675-B8EA-F869FB9C0AA0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A27605-7192-43BC-8FC3-C5F89C0328EC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12972" windowHeight="4992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="119">
   <si>
     <t>Acosta</t>
   </si>
@@ -372,10 +378,16 @@
     <t>VICTIMA_2018</t>
   </si>
   <si>
-    <t>fincas_agro</t>
-  </si>
-  <si>
-    <t>extension_agro</t>
+    <t>Fincas_agro</t>
+  </si>
+  <si>
+    <t>Extension_agro</t>
+  </si>
+  <si>
+    <t>Por_agro</t>
+  </si>
+  <si>
+    <t>Por_menor_15</t>
   </si>
 </sst>
 </file>
@@ -387,7 +399,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +421,10 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -427,12 +443,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -457,12 +474,13 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Millares [0] 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Millares 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Millares 3" xfId="4" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 3" xfId="5" xr:uid="{12AB6F53-9B0E-4434-8DC6-C760D11DEC75}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -740,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ82"/>
+  <dimension ref="A1:AL82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AJ1" sqref="AJ1"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AL2" sqref="AL2:AL82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -754,7 +772,7 @@
     <col min="6" max="34" width="11.44140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>82</v>
       </c>
@@ -863,8 +881,14 @@
       <c r="AJ1" s="6" t="s">
         <v>116</v>
       </c>
+      <c r="AK1" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL1" s="6" t="s">
+        <v>118</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>101</v>
       </c>
@@ -973,8 +997,14 @@
       <c r="AJ2">
         <v>18.2761</v>
       </c>
+      <c r="AK2">
+        <v>0.85299176373526497</v>
+      </c>
+      <c r="AL2">
+        <v>21.6</v>
+      </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>102</v>
       </c>
@@ -1083,8 +1113,14 @@
       <c r="AJ3">
         <v>38.47786</v>
       </c>
+      <c r="AK3">
+        <v>4.0107671601615076</v>
+      </c>
+      <c r="AL3">
+        <v>20.7</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>103</v>
       </c>
@@ -1193,8 +1229,14 @@
       <c r="AJ4">
         <v>4868.5383199999997</v>
       </c>
+      <c r="AK4">
+        <v>3.2989613689008443</v>
+      </c>
+      <c r="AL4">
+        <v>23.6</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>104</v>
       </c>
@@ -1303,8 +1345,14 @@
       <c r="AJ5">
         <v>9813.6080700000002</v>
       </c>
+      <c r="AK5">
+        <v>22.173155142359093</v>
+      </c>
+      <c r="AL5">
+        <v>21.9</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>105</v>
       </c>
@@ -1413,8 +1461,14 @@
       <c r="AJ6">
         <v>9959.7000000000007</v>
       </c>
+      <c r="AK6">
+        <v>52.32974910394266</v>
+      </c>
+      <c r="AL6">
+        <v>27.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>106</v>
       </c>
@@ -1523,8 +1577,14 @@
       <c r="AJ7">
         <v>4010.7341299999998</v>
       </c>
+      <c r="AK7">
+        <v>10.097870652030155</v>
+      </c>
+      <c r="AL7">
+        <v>25</v>
+      </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>107</v>
       </c>
@@ -1633,8 +1693,14 @@
       <c r="AJ8">
         <v>2326.7319000000002</v>
       </c>
+      <c r="AK8">
+        <v>11.842483472262144</v>
+      </c>
+      <c r="AL8">
+        <v>22.4</v>
+      </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>108</v>
       </c>
@@ -1743,8 +1809,14 @@
       <c r="AJ9">
         <v>122.43635</v>
       </c>
+      <c r="AK9">
+        <v>1.4283255893994149</v>
+      </c>
+      <c r="AL9">
+        <v>21.3</v>
+      </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>109</v>
       </c>
@@ -1853,8 +1925,14 @@
       <c r="AJ10">
         <v>1760.6796200000001</v>
       </c>
+      <c r="AK10">
+        <v>4.4484520589119327</v>
+      </c>
+      <c r="AL10">
+        <v>22.4</v>
+      </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>110</v>
       </c>
@@ -1963,8 +2041,14 @@
       <c r="AJ11">
         <v>371.64613000000003</v>
       </c>
+      <c r="AK11">
+        <v>1.0896199363953913</v>
+      </c>
+      <c r="AL11">
+        <v>26.9</v>
+      </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>111</v>
       </c>
@@ -2073,8 +2157,14 @@
       <c r="AJ12">
         <v>45.866999999999997</v>
       </c>
+      <c r="AK12">
+        <v>2.9789864029666253</v>
+      </c>
+      <c r="AL12">
+        <v>21.1</v>
+      </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>112</v>
       </c>
@@ -2183,8 +2273,14 @@
       <c r="AJ13">
         <v>7489.58374</v>
       </c>
+      <c r="AK13">
+        <v>39.242810338551152</v>
+      </c>
+      <c r="AL13">
+        <v>24.4</v>
+      </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>113</v>
       </c>
@@ -2293,8 +2389,14 @@
       <c r="AJ14">
         <v>4.2967000000000004</v>
       </c>
+      <c r="AK14">
+        <v>1.0787154040559699</v>
+      </c>
+      <c r="AL14">
+        <v>19.5</v>
+      </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>114</v>
       </c>
@@ -2403,8 +2505,14 @@
       <c r="AJ15">
         <v>298.14118000000002</v>
       </c>
+      <c r="AK15">
+        <v>2.5066844919786098</v>
+      </c>
+      <c r="AL15">
+        <v>20.2</v>
+      </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>115</v>
       </c>
@@ -2513,8 +2621,14 @@
       <c r="AJ16">
         <v>113.3767</v>
       </c>
+      <c r="AK16">
+        <v>1.593594527363184</v>
+      </c>
+      <c r="AL16">
+        <v>15.4</v>
+      </c>
     </row>
-    <row r="17" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>116</v>
       </c>
@@ -2623,8 +2737,14 @@
       <c r="AJ17">
         <v>5030.68138</v>
       </c>
+      <c r="AK17">
+        <v>40.06666666666667</v>
+      </c>
+      <c r="AL17">
+        <v>25</v>
+      </c>
     </row>
-    <row r="18" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>117</v>
       </c>
@@ -2733,8 +2853,14 @@
       <c r="AJ18">
         <v>7984.7277100000001</v>
       </c>
+      <c r="AK18">
+        <v>57.248677248677247</v>
+      </c>
+      <c r="AL18">
+        <v>25.7</v>
+      </c>
     </row>
-    <row r="19" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>118</v>
       </c>
@@ -2843,8 +2969,14 @@
       <c r="AJ19">
         <v>204.04432</v>
       </c>
+      <c r="AK19">
+        <v>1.8737029350726357</v>
+      </c>
+      <c r="AL19">
+        <v>20.399999999999999</v>
+      </c>
     </row>
-    <row r="20" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>119</v>
       </c>
@@ -2953,8 +3085,14 @@
       <c r="AJ20">
         <v>45514.564279999999</v>
       </c>
+      <c r="AK20">
+        <v>35.972348212330694</v>
+      </c>
+      <c r="AL20">
+        <v>27</v>
+      </c>
     </row>
-    <row r="21" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>120</v>
       </c>
@@ -3063,8 +3201,14 @@
       <c r="AJ21">
         <v>5048.1860500000003</v>
       </c>
+      <c r="AK21">
+        <v>62.061794414735594</v>
+      </c>
+      <c r="AL21">
+        <v>25.5</v>
+      </c>
     </row>
-    <row r="22" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>201</v>
       </c>
@@ -3173,8 +3317,14 @@
       <c r="AJ22">
         <v>7384.2464799999998</v>
       </c>
+      <c r="AK22">
+        <v>7.6226493138138354</v>
+      </c>
+      <c r="AL22">
+        <v>23.5</v>
+      </c>
     </row>
-    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>202</v>
       </c>
@@ -3283,8 +3433,14 @@
       <c r="AJ23">
         <v>13925.193240000001</v>
       </c>
+      <c r="AK23">
+        <v>23.153360419012188</v>
+      </c>
+      <c r="AL23">
+        <v>24.2</v>
+      </c>
     </row>
-    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>203</v>
       </c>
@@ -3393,8 +3549,14 @@
       <c r="AJ24">
         <v>13580.60289</v>
       </c>
+      <c r="AK24">
+        <v>20.931129211046315</v>
+      </c>
+      <c r="AL24">
+        <v>24.3</v>
+      </c>
     </row>
-    <row r="25" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>204</v>
       </c>
@@ -3503,8 +3665,14 @@
       <c r="AJ25">
         <v>2927.0706700000001</v>
       </c>
+      <c r="AK25">
+        <v>40.507936507936506</v>
+      </c>
+      <c r="AL25">
+        <v>23.1</v>
+      </c>
     </row>
-    <row r="26" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>205</v>
       </c>
@@ -3613,8 +3781,14 @@
       <c r="AJ26">
         <v>3512.45579</v>
       </c>
+      <c r="AK26">
+        <v>17.089628869003963</v>
+      </c>
+      <c r="AL26">
+        <v>21.4</v>
+      </c>
     </row>
-    <row r="27" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>206</v>
       </c>
@@ -3723,8 +3897,14 @@
       <c r="AJ27">
         <v>6563.9673700000003</v>
       </c>
+      <c r="AK27">
+        <v>22.436419585482849</v>
+      </c>
+      <c r="AL27">
+        <v>24.4</v>
+      </c>
     </row>
-    <row r="28" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>207</v>
       </c>
@@ -3833,8 +4013,14 @@
       <c r="AJ28">
         <v>1949.3895399999999</v>
       </c>
+      <c r="AK28">
+        <v>13.310314101136111</v>
+      </c>
+      <c r="AL28">
+        <v>22.1</v>
+      </c>
     </row>
-    <row r="29" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>208</v>
       </c>
@@ -3943,8 +4129,14 @@
       <c r="AJ29">
         <v>3592.56097</v>
       </c>
+      <c r="AK29">
+        <v>20.957392197125259</v>
+      </c>
+      <c r="AL29">
+        <v>24.9</v>
+      </c>
     </row>
-    <row r="30" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>209</v>
       </c>
@@ -4053,8 +4245,14 @@
       <c r="AJ30">
         <v>4792.7634600000001</v>
       </c>
+      <c r="AK30">
+        <v>13.403951925035647</v>
+      </c>
+      <c r="AL30">
+        <v>25.6</v>
+      </c>
     </row>
-    <row r="31" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>210</v>
       </c>
@@ -4163,8 +4361,14 @@
       <c r="AJ31">
         <v>67414.28198</v>
       </c>
+      <c r="AK31">
+        <v>33.4061490553322</v>
+      </c>
+      <c r="AL31">
+        <v>28.7</v>
+      </c>
     </row>
-    <row r="32" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>211</v>
       </c>
@@ -4273,8 +4477,14 @@
       <c r="AJ32">
         <v>1172.4636</v>
       </c>
+      <c r="AK32">
+        <v>50.947995666305523</v>
+      </c>
+      <c r="AL32">
+        <v>24.2</v>
+      </c>
     </row>
-    <row r="33" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>212</v>
       </c>
@@ -4383,8 +4593,14 @@
       <c r="AJ33">
         <v>4173.25576</v>
       </c>
+      <c r="AK33">
+        <v>20.711974110032365</v>
+      </c>
+      <c r="AL33">
+        <v>24.6</v>
+      </c>
     </row>
-    <row r="34" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>213</v>
       </c>
@@ -4493,8 +4709,14 @@
       <c r="AJ34">
         <v>27704.539980000001</v>
       </c>
+      <c r="AK34">
+        <v>56.604154063319221</v>
+      </c>
+      <c r="AL34">
+        <v>31.1</v>
+      </c>
     </row>
-    <row r="35" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>214</v>
       </c>
@@ -4603,8 +4825,14 @@
       <c r="AJ35">
         <v>37750.27592</v>
       </c>
+      <c r="AK35">
+        <v>65.825846579129234</v>
+      </c>
+      <c r="AL35">
+        <v>31.8</v>
+      </c>
     </row>
-    <row r="36" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>215</v>
       </c>
@@ -4713,8 +4941,14 @@
       <c r="AJ36">
         <v>12276.34989</v>
       </c>
+      <c r="AK36">
+        <v>59.29133858267717</v>
+      </c>
+      <c r="AL36">
+        <v>29.2</v>
+      </c>
     </row>
-    <row r="37" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>301</v>
       </c>
@@ -4823,8 +5057,14 @@
       <c r="AJ37">
         <v>6102.5852800000002</v>
       </c>
+      <c r="AK37">
+        <v>12.959075240390847</v>
+      </c>
+      <c r="AL37">
+        <v>22.9</v>
+      </c>
     </row>
-    <row r="38" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>302</v>
       </c>
@@ -4933,8 +5173,14 @@
       <c r="AJ38">
         <v>7036.4926100000002</v>
       </c>
+      <c r="AK38">
+        <v>18.764499237754357</v>
+      </c>
+      <c r="AL38">
+        <v>25</v>
+      </c>
     </row>
-    <row r="39" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>303</v>
       </c>
@@ -5043,8 +5289,14 @@
       <c r="AJ39">
         <v>988.90380000000005</v>
       </c>
+      <c r="AK39">
+        <v>2.5328655692200934</v>
+      </c>
+      <c r="AL39">
+        <v>24.5</v>
+      </c>
     </row>
-    <row r="40" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>304</v>
       </c>
@@ -5153,8 +5405,14 @@
       <c r="AJ40">
         <v>6320.2364299999999</v>
       </c>
+      <c r="AK40">
+        <v>39.366989275438137</v>
+      </c>
+      <c r="AL40">
+        <v>23.8</v>
+      </c>
     </row>
-    <row r="41" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>305</v>
       </c>
@@ -5263,8 +5521,14 @@
       <c r="AJ41">
         <v>29475.126950000002</v>
       </c>
+      <c r="AK41">
+        <v>28.154821883705765</v>
+      </c>
+      <c r="AL41">
+        <v>24.3</v>
+      </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>306</v>
       </c>
@@ -5373,8 +5637,14 @@
       <c r="AJ42">
         <v>2229.8932500000001</v>
       </c>
+      <c r="AK42">
+        <v>53.809410078815375</v>
+      </c>
+      <c r="AL42">
+        <v>25.3</v>
+      </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>307</v>
       </c>
@@ -5483,8 +5753,14 @@
       <c r="AJ43">
         <v>2199.4108200000001</v>
       </c>
+      <c r="AK43">
+        <v>26.881631981574401</v>
+      </c>
+      <c r="AL43">
+        <v>25</v>
+      </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>308</v>
       </c>
@@ -5593,8 +5869,14 @@
       <c r="AJ44">
         <v>2160.9303500000001</v>
       </c>
+      <c r="AK44">
+        <v>14.564722368190578</v>
+      </c>
+      <c r="AL44">
+        <v>25.1</v>
+      </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>401</v>
       </c>
@@ -5703,8 +5985,14 @@
       <c r="AJ45">
         <v>1130.15969</v>
       </c>
+      <c r="AK45">
+        <v>1.6413469068128426</v>
+      </c>
+      <c r="AL45">
+        <v>21.6</v>
+      </c>
     </row>
-    <row r="46" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>402</v>
       </c>
@@ -5813,8 +6101,14 @@
       <c r="AJ46">
         <v>1576.2536399999999</v>
       </c>
+      <c r="AK46">
+        <v>5.2655306104048325</v>
+      </c>
+      <c r="AL46">
+        <v>22.3</v>
+      </c>
     </row>
-    <row r="47" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>403</v>
       </c>
@@ -5923,8 +6217,14 @@
       <c r="AJ47">
         <v>1076.1513600000001</v>
       </c>
+      <c r="AK47">
+        <v>3.8365071992568507</v>
+      </c>
+      <c r="AL47">
+        <v>19.899999999999999</v>
+      </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>404</v>
       </c>
@@ -6033,8 +6333,14 @@
       <c r="AJ48">
         <v>1499.6775</v>
       </c>
+      <c r="AK48">
+        <v>7.8362690152121699</v>
+      </c>
+      <c r="AL48">
+        <v>23.6</v>
+      </c>
     </row>
-    <row r="49" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>405</v>
       </c>
@@ -6143,8 +6449,14 @@
       <c r="AJ49">
         <v>773.16048999999998</v>
       </c>
+      <c r="AK49">
+        <v>3.7342703056054907</v>
+      </c>
+      <c r="AL49">
+        <v>22.7</v>
+      </c>
     </row>
-    <row r="50" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>406</v>
       </c>
@@ -6253,8 +6565,14 @@
       <c r="AJ50">
         <v>1014.52535</v>
       </c>
+      <c r="AK50">
+        <v>6.8031933356473449</v>
+      </c>
+      <c r="AL50">
+        <v>21.6</v>
+      </c>
     </row>
-    <row r="51" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>407</v>
       </c>
@@ -6363,8 +6681,14 @@
       <c r="AJ51">
         <v>49.526699999999998</v>
       </c>
+      <c r="AK51">
+        <v>3.739245532759762</v>
+      </c>
+      <c r="AL51">
+        <v>19.2</v>
+      </c>
     </row>
-    <row r="52" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>408</v>
       </c>
@@ -6473,8 +6797,14 @@
       <c r="AJ52">
         <v>77.237260000000006</v>
       </c>
+      <c r="AK52">
+        <v>2.7742288738820955</v>
+      </c>
+      <c r="AL52">
+        <v>21.8</v>
+      </c>
     </row>
-    <row r="53" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>409</v>
       </c>
@@ -6583,8 +6913,14 @@
       <c r="AJ53">
         <v>283.13409000000001</v>
       </c>
+      <c r="AK53">
+        <v>1.8062397372742198</v>
+      </c>
+      <c r="AL53">
+        <v>20.8</v>
+      </c>
     </row>
-    <row r="54" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>410</v>
       </c>
@@ -6693,8 +7029,14 @@
       <c r="AJ54">
         <v>38907.79135</v>
       </c>
+      <c r="AK54">
+        <v>55.863134968032035</v>
+      </c>
+      <c r="AL54">
+        <v>31</v>
+      </c>
     </row>
-    <row r="55" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>501</v>
       </c>
@@ -6803,8 +7145,14 @@
       <c r="AJ55">
         <v>31204.534339999998</v>
       </c>
+      <c r="AK55">
+        <v>12.300764777356871</v>
+      </c>
+      <c r="AL55">
+        <v>27.6</v>
+      </c>
     </row>
-    <row r="56" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>502</v>
       </c>
@@ -6913,8 +7261,14 @@
       <c r="AJ56">
         <v>19418.8969</v>
       </c>
+      <c r="AK56">
+        <v>24.524644637253093</v>
+      </c>
+      <c r="AL56">
+        <v>24</v>
+      </c>
     </row>
-    <row r="57" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>503</v>
       </c>
@@ -7023,8 +7377,14 @@
       <c r="AJ57">
         <v>18398.543399999999</v>
       </c>
+      <c r="AK57">
+        <v>17.85890478539714</v>
+      </c>
+      <c r="AL57">
+        <v>24.4</v>
+      </c>
     </row>
-    <row r="58" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>504</v>
       </c>
@@ -7133,8 +7493,14 @@
       <c r="AJ58">
         <v>13886.555710000001</v>
       </c>
+      <c r="AK58">
+        <v>36.814621409921671</v>
+      </c>
+      <c r="AL58">
+        <v>28.1</v>
+      </c>
     </row>
-    <row r="59" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>505</v>
       </c>
@@ -7243,8 +7609,14 @@
       <c r="AJ59">
         <v>19947.695449999999</v>
       </c>
+      <c r="AK59">
+        <v>18.473396320238688</v>
+      </c>
+      <c r="AL59">
+        <v>26.7</v>
+      </c>
     </row>
-    <row r="60" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>506</v>
       </c>
@@ -7353,8 +7725,14 @@
       <c r="AJ60">
         <v>24708.24955</v>
       </c>
+      <c r="AK60">
+        <v>32.282591477902741</v>
+      </c>
+      <c r="AL60">
+        <v>27.4</v>
+      </c>
     </row>
-    <row r="61" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>507</v>
       </c>
@@ -7463,8 +7841,14 @@
       <c r="AJ61">
         <v>9906.7518099999998</v>
       </c>
+      <c r="AK61">
+        <v>30.515891294334409</v>
+      </c>
+      <c r="AL61">
+        <v>26.1</v>
+      </c>
     </row>
-    <row r="62" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>508</v>
       </c>
@@ -7573,8 +7957,14 @@
       <c r="AJ62">
         <v>1679.0437199999999</v>
       </c>
+      <c r="AK62">
+        <v>26.344193483909656</v>
+      </c>
+      <c r="AL62">
+        <v>25.1</v>
+      </c>
     </row>
-    <row r="63" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>509</v>
       </c>
@@ -7683,8 +8073,14 @@
       <c r="AJ63">
         <v>10735.197700000001</v>
       </c>
+      <c r="AK63">
+        <v>42.716146861429131</v>
+      </c>
+      <c r="AL63">
+        <v>24.6</v>
+      </c>
     </row>
-    <row r="64" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>510</v>
       </c>
@@ -7793,8 +8189,14 @@
       <c r="AJ64">
         <v>27916.789669999998</v>
       </c>
+      <c r="AK64">
+        <v>47.258979206049148</v>
+      </c>
+      <c r="AL64">
+        <v>31.7</v>
+      </c>
     </row>
-    <row r="65" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>511</v>
       </c>
@@ -7903,8 +8305,14 @@
       <c r="AJ65">
         <v>7923.7333699999999</v>
       </c>
+      <c r="AK65">
+        <v>42.32987312572088</v>
+      </c>
+      <c r="AL65">
+        <v>23.3</v>
+      </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>601</v>
       </c>
@@ -8013,8 +8421,14 @@
       <c r="AJ66">
         <v>29401.57763</v>
       </c>
+      <c r="AK66">
+        <v>23.455356139233391</v>
+      </c>
+      <c r="AL66">
+        <v>26.8</v>
+      </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>602</v>
       </c>
@@ -8123,8 +8537,14 @@
       <c r="AJ67">
         <v>2158.4697799999999</v>
       </c>
+      <c r="AK67">
+        <v>10.10562375107051</v>
+      </c>
+      <c r="AL67">
+        <v>25.2</v>
+      </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>603</v>
       </c>
@@ -8233,8 +8653,14 @@
       <c r="AJ68">
         <v>50098.695780000002</v>
       </c>
+      <c r="AK68">
+        <v>65.526740761850476</v>
+      </c>
+      <c r="AL68">
+        <v>32.200000000000003</v>
+      </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>604</v>
       </c>
@@ -8343,8 +8769,14 @@
       <c r="AJ69">
         <v>2510.3966700000001</v>
       </c>
+      <c r="AK69">
+        <v>17.21132897603486</v>
+      </c>
+      <c r="AL69">
+        <v>23.6</v>
+      </c>
     </row>
-    <row r="70" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>605</v>
       </c>
@@ -8453,8 +8885,14 @@
       <c r="AJ70">
         <v>24832.624599999999</v>
       </c>
+      <c r="AK70">
+        <v>35.769125308472717</v>
+      </c>
+      <c r="AL70">
+        <v>27.1</v>
+      </c>
     </row>
-    <row r="71" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>606</v>
       </c>
@@ -8563,8 +9001,14 @@
       <c r="AJ71">
         <v>16672.324000000001</v>
       </c>
+      <c r="AK71">
+        <v>22.258953168044076</v>
+      </c>
+      <c r="AL71">
+        <v>26.3</v>
+      </c>
     </row>
-    <row r="72" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>607</v>
       </c>
@@ -8673,8 +9117,14 @@
       <c r="AJ72">
         <v>20136.60655</v>
       </c>
+      <c r="AK72">
+        <v>31.623564760167401</v>
+      </c>
+      <c r="AL72">
+        <v>28.4</v>
+      </c>
     </row>
-    <row r="73" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>608</v>
       </c>
@@ -8783,8 +9233,14 @@
       <c r="AJ73">
         <v>19620.416980000002</v>
       </c>
+      <c r="AK73">
+        <v>53.652134215932435</v>
+      </c>
+      <c r="AL73">
+        <v>30.4</v>
+      </c>
     </row>
-    <row r="74" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>609</v>
       </c>
@@ -8893,8 +9349,14 @@
       <c r="AJ74">
         <v>12861.6014</v>
       </c>
+      <c r="AK74">
+        <v>30.805463966085728</v>
+      </c>
+      <c r="AL74">
+        <v>26.4</v>
+      </c>
     </row>
-    <row r="75" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>610</v>
       </c>
@@ -9003,8 +9465,14 @@
       <c r="AJ75">
         <v>38577.989300000001</v>
       </c>
+      <c r="AK75">
+        <v>35.571456577141738</v>
+      </c>
+      <c r="AL75">
+        <v>29.3</v>
+      </c>
     </row>
-    <row r="76" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>611</v>
       </c>
@@ -9113,8 +9581,14 @@
       <c r="AJ76">
         <v>4325.4379499999995</v>
       </c>
+      <c r="AK76">
+        <v>10.140237324703344</v>
+      </c>
+      <c r="AL76">
+        <v>28.9</v>
+      </c>
     </row>
-    <row r="77" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>701</v>
       </c>
@@ -9223,8 +9697,14 @@
       <c r="AJ77">
         <v>25077.658780000002</v>
       </c>
+      <c r="AK77">
+        <v>22.735982250907625</v>
+      </c>
+      <c r="AL77">
+        <v>30.6</v>
+      </c>
     </row>
-    <row r="78" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>702</v>
       </c>
@@ -9333,8 +9813,14 @@
       <c r="AJ78">
         <v>40061.07144</v>
       </c>
+      <c r="AK78">
+        <v>44.156424581005588</v>
+      </c>
+      <c r="AL78">
+        <v>28.8</v>
+      </c>
     </row>
-    <row r="79" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>703</v>
       </c>
@@ -9443,8 +9929,14 @@
       <c r="AJ79">
         <v>28128.449509999999</v>
       </c>
+      <c r="AK79">
+        <v>52.542960088691792</v>
+      </c>
+      <c r="AL79">
+        <v>29.3</v>
+      </c>
     </row>
-    <row r="80" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>704</v>
       </c>
@@ -9553,8 +10045,14 @@
       <c r="AJ80">
         <v>26991.2078</v>
       </c>
+      <c r="AK80">
+        <v>58.23546261816098</v>
+      </c>
+      <c r="AL80">
+        <v>35.200000000000003</v>
+      </c>
     </row>
-    <row r="81" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>705</v>
       </c>
@@ -9663,8 +10161,14 @@
       <c r="AJ81">
         <v>16796.59045</v>
       </c>
+      <c r="AK81">
+        <v>71.042550988715192</v>
+      </c>
+      <c r="AL81">
+        <v>31.8</v>
+      </c>
     </row>
-    <row r="82" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>706</v>
       </c>
@@ -9772,6 +10276,12 @@
       </c>
       <c r="AJ82">
         <v>15461.2922</v>
+      </c>
+      <c r="AK82">
+        <v>55.737385544515881</v>
+      </c>
+      <c r="AL82">
+        <v>29.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>